<commit_message>
PR feedback - account for leading 0 as well
</commit_message>
<xml_diff>
--- a/cmd/SplitFFISSpreadsheet/fixtures/example_spreadsheet_four_digit_cfda.xlsx
+++ b/cmd/SplitFFISSpreadsheet/fixtures/example_spreadsheet_four_digit_cfda.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pearkes/code/grants-ingest/cmd/SplitFFISSpreadsheet/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04CDF277-1D36-4070-B044-DDDACD19BB11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F8AD8DC-1F97-447B-A1DE-290C43B8D5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14960" yWindow="7720" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -899,7 +899,7 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="73" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A18" sqref="A18:N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
@@ -1283,9 +1283,9 @@
       <c r="M16" s="43"/>
       <c r="N16" s="37"/>
     </row>
-    <row r="17" spans="1:14" ht="33.950000000000003">
+    <row r="17" spans="1:14" ht="32.25">
       <c r="A17" s="22">
-        <v>10.025</v>
+        <v>2.98</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>31</v>
@@ -1375,15 +1375,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <MigrationWizIdSecurityGroups xmlns="3f8d0ea1-627c-4cbc-a98e-e32c5247faaa" xsi:nil="true"/>
@@ -1406,6 +1397,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1696,11 +1696,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC470876-9485-4376-A615-A485550D2A4F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE4E2C0-647E-49CD-89C3-F903FB174671}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE4E2C0-647E-49CD-89C3-F903FB174671}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC470876-9485-4376-A615-A485550D2A4F}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>